<commit_message>
Milestone 4: fixing bugs
</commit_message>
<xml_diff>
--- a/public/assets/template_export.xlsx
+++ b/public/assets/template_export.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\csv\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\UTC\utcert-web\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C629B51E-E774-415C-8C41-275A399D65A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A41F51F-455B-499C-8B44-C309D3D8CF1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{F5A38BA2-20A7-4194-B90C-B57D29C547DB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Student ID</t>
   </si>
@@ -94,12 +94,6 @@
   </si>
   <si>
     <t>Nguyen Hong Anh</t>
-  </si>
-  <si>
-    <t>Attachment</t>
-  </si>
-  <si>
-    <t>C:\Users\ADMIN\Desktop\csv\bang-diem-demo.xls</t>
   </si>
 </sst>
 </file>
@@ -149,13 +143,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -471,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95FF4CE5-532E-4845-92E6-9D09821CE1F2}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,11 +486,10 @@
     <col min="8" max="8" width="14.42578125" customWidth="1"/>
     <col min="9" max="9" width="18.85546875" customWidth="1"/>
     <col min="10" max="10" width="16.28515625" customWidth="1"/>
-    <col min="11" max="11" width="21.28515625" customWidth="1"/>
-    <col min="12" max="12" width="22" customWidth="1"/>
+    <col min="11" max="11" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -527,11 +523,8 @@
       <c r="K1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>20</v>
-      </c>
     </row>
-    <row r="2" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -562,11 +555,8 @@
       <c r="J2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>